<commit_message>
Fixed R_Value update problem
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -359,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,110 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <f>(C4*100)/B4</f>
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>(E4*100)/B4</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <f>(C5*100)/B5</f>
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>(E5*100)/B5</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>59</v>
+      </c>
+      <c r="D6">
+        <f>(C6*100)/B6</f>
+        <v>59</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <f>(E6*100)/B6</f>
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <v>288</v>
+      </c>
+      <c r="D7">
+        <f>(C7*100)/B7</f>
+        <v>57.6</v>
+      </c>
+      <c r="E7">
+        <v>196</v>
+      </c>
+      <c r="F7">
+        <f>(E7*100)/B7</f>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="G7">
+        <v>97.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>